<commit_message>
Formatacao de Grafico e Linha e Coluna
</commit_message>
<xml_diff>
--- a/7-Gráficos/03. Opções de Formatação de Gráfico (Parte 2) - Material(1).xlsx
+++ b/7-Gráficos/03. Opções de Formatação de Gráfico (Parte 2) - Material(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Excel Impressionador/Módulo 10 - Gráficos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB362B6-3A84-447E-8AF8-8D5FF359ACCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C2DBC8-21A7-43ED-8A01-D43321610CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico de Colunas" sheetId="1" r:id="rId1"/>
@@ -67,12 +67,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Vendas</t>
   </si>
@@ -216,6 +219,9 @@
   </si>
   <si>
     <t>Ano 2020</t>
+  </si>
+  <si>
+    <t>Meta</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -415,11 +421,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,11 +535,131 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -509,6 +670,1141 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10319961042059003"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.86902246302682928"/>
+          <c:h val="0.6315700641586468"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vendas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas'!$B$3:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas'!$C$3:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5977</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9258</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9620</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3177</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B72-426B-A986-A5793B7F56EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="428203983"/>
+        <c:axId val="428204463"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas'!$B$3:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas'!$D$3:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B72-426B-A986-A5793B7F56EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="428203983"/>
+        <c:axId val="428204463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="428203983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428204463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="428204463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428203983"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2000"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>91966</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>24305</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>210207</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100505</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93115E8D-DAC0-A341-BFB4-B12478770993}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F65FBFC8-1F30-45CB-98F1-3E1F9FABD22E}" name="Tabela1" displayName="Tabela1" ref="B2:D13" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="B2:D13" xr:uid="{F65FBFC8-1F30-45CB-98F1-3E1F9FABD22E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A8780D24-8CF5-4325-8509-5E815815B9D4}" name="Mês" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{84CAFF2A-641F-4AE2-BA4C-F8DAB5D99F4E}" name="Vendas" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{43FB5E30-0A52-4317-8675-906A6FB8D20D}" name="Meta" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -774,119 +2070,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="D2" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>5318</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>1692</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>5977</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+      <c r="D5" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>9258</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>8111</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+      <c r="D7" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>4639</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>6895</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+      <c r="D9" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>9620</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+      <c r="D10" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>7443</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+      <c r="D11" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>3177</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
+      <c r="D12" s="33">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>5780</v>
+      </c>
+      <c r="D13" s="33">
+        <v>7500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -898,15 +2234,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
@@ -917,7 +2253,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -928,7 +2264,7 @@
         <v>9344</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -939,7 +2275,7 @@
         <v>6573</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -950,7 +2286,7 @@
         <v>7332</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -961,7 +2297,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -972,7 +2308,7 @@
         <v>5310</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -983,7 +2319,7 @@
         <v>9395</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -994,7 +2330,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +2341,7 @@
         <v>9455</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +2352,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1027,7 +2363,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +2374,7 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1061,25 +2397,25 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="107" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="6.54296875" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="6"/>
+    <col min="3" max="3" width="6.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="6.5703125" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="D3" s="16" t="s">
         <v>37</v>
@@ -1091,7 +2427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
       <c r="D4" s="8" t="s">
         <v>35</v>
@@ -1103,7 +2439,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
@@ -1117,7 +2453,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1131,7 +2467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
@@ -1145,7 +2481,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +2495,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13"/>
       <c r="D9" s="8" t="s">
         <v>26</v>
@@ -1171,7 +2507,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
@@ -1185,7 +2521,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
@@ -1199,7 +2535,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +2549,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="D13" s="8" t="s">
         <v>19</v>
@@ -1225,7 +2561,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>18</v>
       </c>
@@ -1239,7 +2575,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1253,12 +2589,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:B3"/>
@@ -1274,16 +2610,16 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="73.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>45</v>
       </c>
@@ -1327,7 +2663,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="29"/>
       <c r="D3" s="25" t="s">
         <v>44</v>
@@ -1369,7 +2705,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="29"/>
       <c r="D4" s="23" t="s">
         <v>42</v>
@@ -1411,7 +2747,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="21" t="s">
         <v>40</v>
       </c>
@@ -1452,17 +2788,17 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>39</v>
       </c>
@@ -1480,7 +2816,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
     </row>
-    <row r="9" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gráfico Combinado e Gráfico de Colunas Agrupadas
</commit_message>
<xml_diff>
--- a/7-Gráficos/03. Opções de Formatação de Gráfico (Parte 2) - Material(1).xlsx
+++ b/7-Gráficos/03. Opções de Formatação de Gráfico (Parte 2) - Material(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C2DBC8-21A7-43ED-8A01-D43321610CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73BEDBA-EF49-4A87-A084-7510B978BD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico de Colunas" sheetId="1" r:id="rId1"/>
@@ -529,12 +529,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -545,6 +539,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,13 +638,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -654,6 +647,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1211,6 +1211,1316 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vendas 2019 x 2020</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ano 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$B$3:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5977</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9258</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9620</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3177</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5780</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6380</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F5C-4AAF-8BFD-1A460FA75F75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ano 2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$B$3:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Agrupadas'!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9344</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6573</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5310</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4487</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9455</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2107</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4353</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F5C-4AAF-8BFD-1A460FA75F75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-27"/>
+        <c:axId val="187430832"/>
+        <c:axId val="187424592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="187430832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="187424592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="187424592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="187430832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent2"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" dir="10800000" algn="r" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vendas x Devoluções</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8678079756159513E-2"/>
+          <c:y val="8.7763643100188235E-2"/>
+          <c:w val="0.91239718906104483"/>
+          <c:h val="0.76912580288317656"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Eixo Secundário'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vendas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Eixo Secundário'!$D$4:$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2015.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2018.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2019.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Eixo Secundário'!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5690</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5990</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10460</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10780</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12210</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A6CA-46A3-8119-411C0B015793}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="228686384"/>
+        <c:axId val="228685904"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Eixo Secundário'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Devoluções</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Eixo Secundário'!$F$4:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>410</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A6CA-46A3-8119-411C0B015793}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="270733888"/>
+        <c:axId val="270745888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="228686384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="228685904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="228685904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="228686384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="270745888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="270733888"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="270733888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="270745888"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1251,7 +2561,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1795,8 +4191,90 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>145073</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>282086</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30773</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C61102C-E0FB-A3FF-548B-6A78D6FE9D7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20E6712-803D-6309-2010-40FB6267BD90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F65FBFC8-1F30-45CB-98F1-3E1F9FABD22E}" name="Tabela1" displayName="Tabela1" ref="B2:D13" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F65FBFC8-1F30-45CB-98F1-3E1F9FABD22E}" name="Tabela1" displayName="Tabela1" ref="B2:D13" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="B2:D13" xr:uid="{F65FBFC8-1F30-45CB-98F1-3E1F9FABD22E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A8780D24-8CF5-4325-8509-5E815815B9D4}" name="Mês" dataDxfId="2"/>
@@ -2072,7 +4550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
@@ -2085,134 +4563,134 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="31" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>5318</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>1692</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>5977</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>9258</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>8111</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>4639</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>6895</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>9620</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>7443</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>3177</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="31">
         <v>7500</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="30" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>5780</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="31">
         <v>7500</v>
       </c>
     </row>
@@ -2231,7 +4709,7 @@
   <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,6 +4866,7 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2395,7 +4874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9466A54-5353-412D-BA0C-0F8BE7522934}">
   <dimension ref="B1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2411,12 +4892,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
+      <c r="B3" s="32"/>
       <c r="D3" s="16" t="s">
         <v>37</v>
       </c>
@@ -2601,6 +5082,7 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2620,7 +5102,7 @@
   <sheetData>
     <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="27" t="s">
@@ -2664,7 +5146,7 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
+      <c r="B3" s="33"/>
       <c r="D3" s="25" t="s">
         <v>44</v>
       </c>
@@ -2706,7 +5188,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
+      <c r="B4" s="33"/>
       <c r="D4" s="23" t="s">
         <v>42</v>
       </c>

</xml_diff>